<commit_message>
Added ngrams, overrhauled Preprocess
</commit_message>
<xml_diff>
--- a/src/weights/NOUN.xlsx
+++ b/src/weights/NOUN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4207,6 +4207,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>